<commit_message>
Variable 'Ost_West_Ausland' in Tabelle 'Postleitzahlen' eingefuegt. setUp- und TearDown-Funktion aktualisiert und alle Unittests daran angepasst. Unittest fuer erfolgreichen Mitarbeiter-Import geschrieben. Alle Tests laufen.
</commit_message>
<xml_diff>
--- a/src/test/testdaten_insert_abteilung/Abteilung.xlsx
+++ b/src/test/testdaten_insert_abteilung/Abteilung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert personenbezogene Daten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\test\testdaten_insert_abteilung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BC8945-C4DD-4784-BADB-54F3A267E52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A372E1D4-B000-4B36-9C3B-5B0199672E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33705" yWindow="1995" windowWidth="17280" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33405" yWindow="3075" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>

</xml_diff>